<commit_message>
Fix to hero name excel file
</commit_message>
<xml_diff>
--- a/Hero Format.xlsx
+++ b/Hero Format.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="291" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="146" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="226">
   <si>
-    <t>npc_dota_hero_antimage</t>
+    <t>Hero: npc_dota_hero_antimage</t>
   </si>
   <si>
     <t>ID: 1</t>
@@ -707,6 +707,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -727,6 +728,7 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -803,8 +805,8 @@
   </sheetPr>
   <dimension ref="A1:C226"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A222" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B225" activeCellId="0" sqref="B225"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A205" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1:B226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -818,17 +820,17 @@
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A1  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A2,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'npc_dota_hero_antimage',1);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A1,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A2,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'antimage',1);</v>
       </c>
       <c r="C1" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A1  &amp; CHAR(39) &amp; "," &amp; RIGHT($A2,1) &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'npc_dota_hero_antimage',1);</v>
+        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_antimage',1);</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -836,7 +838,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A2  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A3,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A2,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A3,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C2" s="2" t="str">
@@ -849,8 +851,8 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A3  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A4,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_axe',2);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A3,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A4,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'axe',2);</v>
       </c>
       <c r="C3" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A3  &amp; CHAR(39) &amp; "," &amp; RIGHT($A4,1) &amp; ");","")</f>
@@ -862,7 +864,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A4  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A5,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A4,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A5,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C4" s="2" t="str">
@@ -875,8 +877,8 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A5  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A6,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_bane',3);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A5,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A6,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'bane',3);</v>
       </c>
       <c r="C5" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A5  &amp; CHAR(39) &amp; "," &amp; RIGHT($A6,1) &amp; ");","")</f>
@@ -888,7 +890,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A6  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A7,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A6,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A7,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C6" s="2" t="str">
@@ -901,8 +903,8 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A7  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A8,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_bloodseeker',4);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A7,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A8,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'bloodseeker',4);</v>
       </c>
       <c r="C7" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A7  &amp; CHAR(39) &amp; "," &amp; RIGHT($A8,1) &amp; ");","")</f>
@@ -914,7 +916,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A8  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A9,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A8,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A9,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C8" s="2" t="str">
@@ -927,8 +929,8 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A9  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A10,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_crystal_maiden',5);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A9,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A10,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'crystal_maiden',5);</v>
       </c>
       <c r="C9" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A9  &amp; CHAR(39) &amp; "," &amp; RIGHT($A10,1) &amp; ");","")</f>
@@ -940,7 +942,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A10  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A11,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A10,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A11,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C10" s="2" t="str">
@@ -953,8 +955,8 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A11  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A12,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_drow_ranger',6);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A11,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A12,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'drow_ranger',6);</v>
       </c>
       <c r="C11" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A11  &amp; CHAR(39) &amp; "," &amp; RIGHT($A12,1) &amp; ");","")</f>
@@ -966,7 +968,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A12  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A13,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A12,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A13,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C12" s="2" t="str">
@@ -979,8 +981,8 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A13  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A14,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_earthshaker',7);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A13,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A14,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'earthshaker',7);</v>
       </c>
       <c r="C13" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A13  &amp; CHAR(39) &amp; "," &amp; RIGHT($A14,1) &amp; ");","")</f>
@@ -992,7 +994,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A14  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A15,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A14,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A15,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C14" s="2" t="str">
@@ -1005,8 +1007,8 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A15  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A16,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_juggernaut',8);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A15,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A16,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'juggernaut',8);</v>
       </c>
       <c r="C15" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A15  &amp; CHAR(39) &amp; "," &amp; RIGHT($A16,1) &amp; ");","")</f>
@@ -1018,7 +1020,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A16  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A17,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A16,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A17,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C16" s="2" t="str">
@@ -1031,8 +1033,8 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A17  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A18,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_mirana',9);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A17,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A18,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'mirana',9);</v>
       </c>
       <c r="C17" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A17  &amp; CHAR(39) &amp; "," &amp; RIGHT($A18,1) &amp; ");","")</f>
@@ -1044,7 +1046,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A18  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A19,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A18,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A19,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C18" s="2" t="str">
@@ -1057,8 +1059,8 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A19  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A20,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_nevermore',11);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A19,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A20,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'nevermore',11);</v>
       </c>
       <c r="C19" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A19  &amp; CHAR(39) &amp; "," &amp; RIGHT($A20,1) &amp; ");","")</f>
@@ -1070,7 +1072,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A20  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A21,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A20,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A21,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C20" s="2" t="str">
@@ -1083,8 +1085,8 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A21  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A22,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_morphling',10);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A21,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A22,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'morphling',10);</v>
       </c>
       <c r="C21" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A21  &amp; CHAR(39) &amp; "," &amp; RIGHT($A22,1) &amp; ");","")</f>
@@ -1096,7 +1098,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A22  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A23,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A22,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A23,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C22" s="2" t="str">
@@ -1109,8 +1111,8 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A23  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A24,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_phantom_lancer',12);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A23,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A24,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'phantom_lancer',12);</v>
       </c>
       <c r="C23" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A23  &amp; CHAR(39) &amp; "," &amp; RIGHT($A24,1) &amp; ");","")</f>
@@ -1122,7 +1124,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A24  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A25,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A24,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A25,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C24" s="2" t="str">
@@ -1135,8 +1137,8 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A25  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A26,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_puck',13);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A25,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A26,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'puck',13);</v>
       </c>
       <c r="C25" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A25  &amp; CHAR(39) &amp; "," &amp; RIGHT($A26,1) &amp; ");","")</f>
@@ -1148,7 +1150,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A26  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A27,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A26,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A27,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C26" s="2" t="str">
@@ -1161,8 +1163,8 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A27  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A28,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_pudge',14);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A27,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A28,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'pudge',14);</v>
       </c>
       <c r="C27" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A27  &amp; CHAR(39) &amp; "," &amp; RIGHT($A28,1) &amp; ");","")</f>
@@ -1174,7 +1176,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A28  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A29,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A28,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A29,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C28" s="2" t="str">
@@ -1187,8 +1189,8 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A29  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A30,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_razor',15);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A29,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A30,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'razor',15);</v>
       </c>
       <c r="C29" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A29  &amp; CHAR(39) &amp; "," &amp; RIGHT($A30,1) &amp; ");","")</f>
@@ -1200,7 +1202,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A30  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A31,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A30,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A31,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C30" s="2" t="str">
@@ -1213,8 +1215,8 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A31  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A32,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_sand_king',16);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A31,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A32,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'sand_king',16);</v>
       </c>
       <c r="C31" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A31  &amp; CHAR(39) &amp; "," &amp; RIGHT($A32,1) &amp; ");","")</f>
@@ -1226,7 +1228,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A32  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A33,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A32,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A33,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C32" s="2" t="str">
@@ -1239,8 +1241,8 @@
         <v>32</v>
       </c>
       <c r="B33" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A33  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A34,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_storm_spirit',17);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A33,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A34,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'storm_spirit',17);</v>
       </c>
       <c r="C33" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A33  &amp; CHAR(39) &amp; "," &amp; RIGHT($A34,1) &amp; ");","")</f>
@@ -1252,7 +1254,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A34  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A35,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A34,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A35,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C34" s="2" t="str">
@@ -1265,8 +1267,8 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A35  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A36,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_sven',18);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A35,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A36,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'sven',18);</v>
       </c>
       <c r="C35" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A35  &amp; CHAR(39) &amp; "," &amp; RIGHT($A36,1) &amp; ");","")</f>
@@ -1278,7 +1280,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A36  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A37,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A36,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A37,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C36" s="2" t="str">
@@ -1291,8 +1293,8 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A37  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A38,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_tiny',19);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A37,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A38,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'tiny',19);</v>
       </c>
       <c r="C37" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A37  &amp; CHAR(39) &amp; "," &amp; RIGHT($A38,1) &amp; ");","")</f>
@@ -1304,7 +1306,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A38  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A39,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A38,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A39,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C38" s="2" t="str">
@@ -1317,8 +1319,8 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A39  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A40,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_vengefulspirit',20);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A39,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A40,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'vengefulspirit',20);</v>
       </c>
       <c r="C39" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A39  &amp; CHAR(39) &amp; "," &amp; RIGHT($A40,1) &amp; ");","")</f>
@@ -1330,7 +1332,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A40  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A41,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A40,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A41,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C40" s="2" t="str">
@@ -1343,8 +1345,8 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A41  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A42,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_windrunner',21);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A41,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A42,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'windrunner',21);</v>
       </c>
       <c r="C41" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A41  &amp; CHAR(39) &amp; "," &amp; RIGHT($A42,1) &amp; ");","")</f>
@@ -1356,7 +1358,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A42  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A43,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A42,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A43,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C42" s="2" t="str">
@@ -1369,8 +1371,8 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A43  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A44,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_zuus',22);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A43,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A44,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'zuus',22);</v>
       </c>
       <c r="C43" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A43  &amp; CHAR(39) &amp; "," &amp; RIGHT($A44,1) &amp; ");","")</f>
@@ -1382,7 +1384,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A44  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A45,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A44,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A45,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C44" s="2" t="str">
@@ -1395,8 +1397,8 @@
         <v>44</v>
       </c>
       <c r="B45" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A45  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A46,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_kunkka',23);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A45,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A46,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'kunkka',23);</v>
       </c>
       <c r="C45" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A45  &amp; CHAR(39) &amp; "," &amp; RIGHT($A46,1) &amp; ");","")</f>
@@ -1408,7 +1410,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A46  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A47,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A46,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A47,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C46" s="2" t="str">
@@ -1421,8 +1423,8 @@
         <v>46</v>
       </c>
       <c r="B47" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A47  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A48,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_lina',25);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A47,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A48,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'lina',25);</v>
       </c>
       <c r="C47" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A47  &amp; CHAR(39) &amp; "," &amp; RIGHT($A48,1) &amp; ");","")</f>
@@ -1434,7 +1436,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A48  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A49,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A48,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A49,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C48" s="2" t="str">
@@ -1447,8 +1449,8 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A49  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A50,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_lich',31);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A49,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A50,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'lich',31);</v>
       </c>
       <c r="C49" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A49  &amp; CHAR(39) &amp; "," &amp; RIGHT($A50,1) &amp; ");","")</f>
@@ -1460,7 +1462,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A50  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A51,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A50,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A51,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C50" s="2" t="str">
@@ -1473,8 +1475,8 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A51  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A52,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_lion',26);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A51,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A52,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'lion',26);</v>
       </c>
       <c r="C51" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A51  &amp; CHAR(39) &amp; "," &amp; RIGHT($A52,1) &amp; ");","")</f>
@@ -1486,7 +1488,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A52  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A53,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A52,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A53,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C52" s="2" t="str">
@@ -1499,8 +1501,8 @@
         <v>52</v>
       </c>
       <c r="B53" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A53  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A54,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_shadow_shaman',27);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A53,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A54,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'shadow_shaman',27);</v>
       </c>
       <c r="C53" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A53  &amp; CHAR(39) &amp; "," &amp; RIGHT($A54,1) &amp; ");","")</f>
@@ -1512,7 +1514,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A54  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A55,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A54,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A55,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C54" s="2" t="str">
@@ -1525,8 +1527,8 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A55  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A56,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_slardar',28);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A55,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A56,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'slardar',28);</v>
       </c>
       <c r="C55" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A55  &amp; CHAR(39) &amp; "," &amp; RIGHT($A56,1) &amp; ");","")</f>
@@ -1538,7 +1540,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A56  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A57,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A56,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A57,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C56" s="2" t="str">
@@ -1551,8 +1553,8 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A57  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A58,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_tidehunter',29);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A57,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A58,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'tidehunter',29);</v>
       </c>
       <c r="C57" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A57  &amp; CHAR(39) &amp; "," &amp; RIGHT($A58,1) &amp; ");","")</f>
@@ -1564,7 +1566,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A58  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A59,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A58,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A59,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C58" s="2" t="str">
@@ -1577,8 +1579,8 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A59  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A60,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_witch_doctor',30);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A59,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A60,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'witch_doctor',30);</v>
       </c>
       <c r="C59" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A59  &amp; CHAR(39) &amp; "," &amp; RIGHT($A60,1) &amp; ");","")</f>
@@ -1590,7 +1592,7 @@
         <v>59</v>
       </c>
       <c r="B60" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A60  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A61,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A60,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A61,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C60" s="2" t="str">
@@ -1603,8 +1605,8 @@
         <v>60</v>
       </c>
       <c r="B61" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A61  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A62,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_riki',32);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A61,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A62,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'riki',32);</v>
       </c>
       <c r="C61" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A61  &amp; CHAR(39) &amp; "," &amp; RIGHT($A62,1) &amp; ");","")</f>
@@ -1616,7 +1618,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A62  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A63,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A62,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A63,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C62" s="2" t="str">
@@ -1629,8 +1631,8 @@
         <v>62</v>
       </c>
       <c r="B63" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A63  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A64,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_enigma',33);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A63,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A64,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'enigma',33);</v>
       </c>
       <c r="C63" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A63  &amp; CHAR(39) &amp; "," &amp; RIGHT($A64,1) &amp; ");","")</f>
@@ -1642,7 +1644,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A64  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A65,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A64,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A65,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C64" s="2" t="str">
@@ -1655,8 +1657,8 @@
         <v>64</v>
       </c>
       <c r="B65" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A65  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A66,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_tinker',34);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A65,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A66,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'tinker',34);</v>
       </c>
       <c r="C65" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A65  &amp; CHAR(39) &amp; "," &amp; RIGHT($A66,1) &amp; ");","")</f>
@@ -1668,7 +1670,7 @@
         <v>65</v>
       </c>
       <c r="B66" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A66  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A67,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A66,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A67,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C66" s="2" t="str">
@@ -1681,8 +1683,8 @@
         <v>66</v>
       </c>
       <c r="B67" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A67  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A68,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_sniper',35);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A67,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A68,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'sniper',35);</v>
       </c>
       <c r="C67" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A67  &amp; CHAR(39) &amp; "," &amp; RIGHT($A68,1) &amp; ");","")</f>
@@ -1694,7 +1696,7 @@
         <v>67</v>
       </c>
       <c r="B68" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A68  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A69,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A68,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A69,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C68" s="2" t="str">
@@ -1707,8 +1709,8 @@
         <v>68</v>
       </c>
       <c r="B69" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A69  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A70,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_necrolyte',36);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A69,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A70,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'necrolyte',36);</v>
       </c>
       <c r="C69" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A69  &amp; CHAR(39) &amp; "," &amp; RIGHT($A70,1) &amp; ");","")</f>
@@ -1720,7 +1722,7 @@
         <v>69</v>
       </c>
       <c r="B70" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A70  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A71,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A70,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A71,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C70" s="2" t="str">
@@ -1733,8 +1735,8 @@
         <v>70</v>
       </c>
       <c r="B71" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A71  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A72,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_warlock',37);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A71,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A72,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'warlock',37);</v>
       </c>
       <c r="C71" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A71  &amp; CHAR(39) &amp; "," &amp; RIGHT($A72,1) &amp; ");","")</f>
@@ -1746,7 +1748,7 @@
         <v>71</v>
       </c>
       <c r="B72" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A72  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A73,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A72,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A73,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C72" s="2" t="str">
@@ -1759,8 +1761,8 @@
         <v>72</v>
       </c>
       <c r="B73" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A73  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A74,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_beastmaster',38);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A73,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A74,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'beastmaster',38);</v>
       </c>
       <c r="C73" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A73  &amp; CHAR(39) &amp; "," &amp; RIGHT($A74,1) &amp; ");","")</f>
@@ -1772,7 +1774,7 @@
         <v>73</v>
       </c>
       <c r="B74" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A74  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A75,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A74,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A75,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C74" s="2" t="str">
@@ -1785,8 +1787,8 @@
         <v>74</v>
       </c>
       <c r="B75" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A75  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A76,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_queenofpain',39);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A75,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A76,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'queenofpain',39);</v>
       </c>
       <c r="C75" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A75  &amp; CHAR(39) &amp; "," &amp; RIGHT($A76,1) &amp; ");","")</f>
@@ -1798,7 +1800,7 @@
         <v>75</v>
       </c>
       <c r="B76" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A76  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A77,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A76,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A77,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C76" s="2" t="str">
@@ -1811,8 +1813,8 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A77  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A78,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_venomancer',40);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A77,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A78,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'venomancer',40);</v>
       </c>
       <c r="C77" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A77  &amp; CHAR(39) &amp; "," &amp; RIGHT($A78,1) &amp; ");","")</f>
@@ -1824,7 +1826,7 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A78  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A79,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A78,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A79,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C78" s="2" t="str">
@@ -1837,8 +1839,8 @@
         <v>78</v>
       </c>
       <c r="B79" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A79  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A80,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_faceless_void',41);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A79,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A80,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'faceless_void',41);</v>
       </c>
       <c r="C79" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A79  &amp; CHAR(39) &amp; "," &amp; RIGHT($A80,1) &amp; ");","")</f>
@@ -1850,7 +1852,7 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A80  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A81,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A80,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A81,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C80" s="2" t="str">
@@ -1863,8 +1865,8 @@
         <v>80</v>
       </c>
       <c r="B81" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A81  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A82,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_skeleton_king',42);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A81,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A82,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'skeleton_king',42);</v>
       </c>
       <c r="C81" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A81  &amp; CHAR(39) &amp; "," &amp; RIGHT($A82,1) &amp; ");","")</f>
@@ -1876,7 +1878,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A82  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A83,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A82,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A83,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C82" s="2" t="str">
@@ -1889,8 +1891,8 @@
         <v>82</v>
       </c>
       <c r="B83" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A83  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A84,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_death_prophet',43);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A83,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A84,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'death_prophet',43);</v>
       </c>
       <c r="C83" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A83  &amp; CHAR(39) &amp; "," &amp; RIGHT($A84,1) &amp; ");","")</f>
@@ -1902,7 +1904,7 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A84  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A85,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A84,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A85,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C84" s="2" t="str">
@@ -1915,8 +1917,8 @@
         <v>84</v>
       </c>
       <c r="B85" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A85  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A86,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_phantom_assassin',44);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A85,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A86,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'phantom_assassin',44);</v>
       </c>
       <c r="C85" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A85  &amp; CHAR(39) &amp; "," &amp; RIGHT($A86,1) &amp; ");","")</f>
@@ -1928,7 +1930,7 @@
         <v>85</v>
       </c>
       <c r="B86" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A86  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A87,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A86,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A87,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C86" s="2" t="str">
@@ -1941,8 +1943,8 @@
         <v>86</v>
       </c>
       <c r="B87" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A87  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A88,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_pugna',45);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A87,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A88,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'pugna',45);</v>
       </c>
       <c r="C87" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A87  &amp; CHAR(39) &amp; "," &amp; RIGHT($A88,1) &amp; ");","")</f>
@@ -1954,7 +1956,7 @@
         <v>87</v>
       </c>
       <c r="B88" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A88  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A89,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A88,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A89,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C88" s="2" t="str">
@@ -1967,8 +1969,8 @@
         <v>88</v>
       </c>
       <c r="B89" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A89  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A90,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_templar_assassin',46);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A89,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A90,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'templar_assassin',46);</v>
       </c>
       <c r="C89" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A89  &amp; CHAR(39) &amp; "," &amp; RIGHT($A90,1) &amp; ");","")</f>
@@ -1980,7 +1982,7 @@
         <v>89</v>
       </c>
       <c r="B90" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A90  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A91,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A90,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A91,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C90" s="2" t="str">
@@ -1993,8 +1995,8 @@
         <v>90</v>
       </c>
       <c r="B91" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A91  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A92,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_viper',47);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A91,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A92,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'viper',47);</v>
       </c>
       <c r="C91" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A91  &amp; CHAR(39) &amp; "," &amp; RIGHT($A92,1) &amp; ");","")</f>
@@ -2006,7 +2008,7 @@
         <v>91</v>
       </c>
       <c r="B92" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A92  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A93,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A92,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A93,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C92" s="2" t="str">
@@ -2019,8 +2021,8 @@
         <v>92</v>
       </c>
       <c r="B93" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A93  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A94,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_luna',48);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A93,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A94,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'luna',48);</v>
       </c>
       <c r="C93" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A93  &amp; CHAR(39) &amp; "," &amp; RIGHT($A94,1) &amp; ");","")</f>
@@ -2032,7 +2034,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A94  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A95,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A94,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A95,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C94" s="2" t="str">
@@ -2045,8 +2047,8 @@
         <v>94</v>
       </c>
       <c r="B95" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A95  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A96,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_dragon_knight',49);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A95,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A96,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'dragon_knight',49);</v>
       </c>
       <c r="C95" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A95  &amp; CHAR(39) &amp; "," &amp; RIGHT($A96,1) &amp; ");","")</f>
@@ -2058,7 +2060,7 @@
         <v>95</v>
       </c>
       <c r="B96" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A96  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A97,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A96,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A97,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C96" s="2" t="str">
@@ -2071,8 +2073,8 @@
         <v>96</v>
       </c>
       <c r="B97" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A97  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A98,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_dazzle',50);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A97,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A98,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'dazzle',50);</v>
       </c>
       <c r="C97" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A97  &amp; CHAR(39) &amp; "," &amp; RIGHT($A98,1) &amp; ");","")</f>
@@ -2084,7 +2086,7 @@
         <v>97</v>
       </c>
       <c r="B98" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A98  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A99,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A98,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A99,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C98" s="2" t="str">
@@ -2097,8 +2099,8 @@
         <v>98</v>
       </c>
       <c r="B99" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A99  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A100,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_rattletrap',51);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A99,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A100,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'rattletrap',51);</v>
       </c>
       <c r="C99" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A99  &amp; CHAR(39) &amp; "," &amp; RIGHT($A100,1) &amp; ");","")</f>
@@ -2110,7 +2112,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A100  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A101,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A100,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A101,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C100" s="2" t="str">
@@ -2123,8 +2125,8 @@
         <v>100</v>
       </c>
       <c r="B101" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A101  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A102,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_leshrac',52);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A101,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A102,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'leshrac',52);</v>
       </c>
       <c r="C101" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A101  &amp; CHAR(39) &amp; "," &amp; RIGHT($A102,1) &amp; ");","")</f>
@@ -2136,7 +2138,7 @@
         <v>101</v>
       </c>
       <c r="B102" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A102  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A103,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A102,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A103,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C102" s="2" t="str">
@@ -2149,8 +2151,8 @@
         <v>102</v>
       </c>
       <c r="B103" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A103  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A104,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_furion',53);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A103,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A104,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'furion',53);</v>
       </c>
       <c r="C103" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A103  &amp; CHAR(39) &amp; "," &amp; RIGHT($A104,1) &amp; ");","")</f>
@@ -2162,7 +2164,7 @@
         <v>103</v>
       </c>
       <c r="B104" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A104  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A105,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A104,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A105,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C104" s="2" t="str">
@@ -2175,8 +2177,8 @@
         <v>104</v>
       </c>
       <c r="B105" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A105  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A106,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_life_stealer',54);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A105,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A106,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'life_stealer',54);</v>
       </c>
       <c r="C105" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A105  &amp; CHAR(39) &amp; "," &amp; RIGHT($A106,1) &amp; ");","")</f>
@@ -2188,7 +2190,7 @@
         <v>105</v>
       </c>
       <c r="B106" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A106  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A107,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A106,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A107,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C106" s="2" t="str">
@@ -2201,8 +2203,8 @@
         <v>106</v>
       </c>
       <c r="B107" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A107  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A108,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_dark_seer',55);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A107,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A108,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'dark_seer',55);</v>
       </c>
       <c r="C107" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A107  &amp; CHAR(39) &amp; "," &amp; RIGHT($A108,1) &amp; ");","")</f>
@@ -2214,7 +2216,7 @@
         <v>107</v>
       </c>
       <c r="B108" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A108  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A109,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A108,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A109,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C108" s="2" t="str">
@@ -2227,8 +2229,8 @@
         <v>108</v>
       </c>
       <c r="B109" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A109  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A110,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_clinkz',56);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A109,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A110,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'clinkz',56);</v>
       </c>
       <c r="C109" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A109  &amp; CHAR(39) &amp; "," &amp; RIGHT($A110,1) &amp; ");","")</f>
@@ -2240,7 +2242,7 @@
         <v>109</v>
       </c>
       <c r="B110" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A110  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A111,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A110,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A111,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C110" s="2" t="str">
@@ -2253,8 +2255,8 @@
         <v>110</v>
       </c>
       <c r="B111" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A111  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A112,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_omniknight',57);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A111,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A112,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'omniknight',57);</v>
       </c>
       <c r="C111" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A111  &amp; CHAR(39) &amp; "," &amp; RIGHT($A112,1) &amp; ");","")</f>
@@ -2266,7 +2268,7 @@
         <v>111</v>
       </c>
       <c r="B112" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A112  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A113,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A112,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A113,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C112" s="2" t="str">
@@ -2279,8 +2281,8 @@
         <v>112</v>
       </c>
       <c r="B113" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A113  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A114,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_enchantress',58);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A113,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A114,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'enchantress',58);</v>
       </c>
       <c r="C113" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A113  &amp; CHAR(39) &amp; "," &amp; RIGHT($A114,1) &amp; ");","")</f>
@@ -2292,7 +2294,7 @@
         <v>113</v>
       </c>
       <c r="B114" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A114  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A115,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A114,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A115,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C114" s="2" t="str">
@@ -2305,8 +2307,8 @@
         <v>114</v>
       </c>
       <c r="B115" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A115  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A116,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_huskar',59);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A115,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A116,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'huskar',59);</v>
       </c>
       <c r="C115" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A115  &amp; CHAR(39) &amp; "," &amp; RIGHT($A116,1) &amp; ");","")</f>
@@ -2318,7 +2320,7 @@
         <v>115</v>
       </c>
       <c r="B116" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A116  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A117,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A116,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A117,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C116" s="2" t="str">
@@ -2331,8 +2333,8 @@
         <v>116</v>
       </c>
       <c r="B117" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A117  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A118,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_night_stalker',60);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A117,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A118,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'night_stalker',60);</v>
       </c>
       <c r="C117" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A117  &amp; CHAR(39) &amp; "," &amp; RIGHT($A118,1) &amp; ");","")</f>
@@ -2344,7 +2346,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A118  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A119,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A118,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A119,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C118" s="2" t="str">
@@ -2357,8 +2359,8 @@
         <v>118</v>
       </c>
       <c r="B119" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A119  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A120,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_broodmother',61);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A119,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A120,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'broodmother',61);</v>
       </c>
       <c r="C119" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A119  &amp; CHAR(39) &amp; "," &amp; RIGHT($A120,1) &amp; ");","")</f>
@@ -2370,7 +2372,7 @@
         <v>119</v>
       </c>
       <c r="B120" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A120  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A121,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A120,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A121,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C120" s="2" t="str">
@@ -2383,8 +2385,8 @@
         <v>120</v>
       </c>
       <c r="B121" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A121  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A122,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_bounty_hunter',62);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A121,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A122,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'bounty_hunter',62);</v>
       </c>
       <c r="C121" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A121  &amp; CHAR(39) &amp; "," &amp; RIGHT($A122,1) &amp; ");","")</f>
@@ -2396,7 +2398,7 @@
         <v>121</v>
       </c>
       <c r="B122" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A122  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A123,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A122,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A123,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C122" s="2" t="str">
@@ -2409,8 +2411,8 @@
         <v>122</v>
       </c>
       <c r="B123" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A123  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A124,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_weaver',63);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A123,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A124,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'weaver',63);</v>
       </c>
       <c r="C123" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A123  &amp; CHAR(39) &amp; "," &amp; RIGHT($A124,1) &amp; ");","")</f>
@@ -2422,7 +2424,7 @@
         <v>123</v>
       </c>
       <c r="B124" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A124  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A125,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A124,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A125,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C124" s="2" t="str">
@@ -2435,8 +2437,8 @@
         <v>124</v>
       </c>
       <c r="B125" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A125  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A126,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_jakiro',64);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A125,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A126,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'jakiro',64);</v>
       </c>
       <c r="C125" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A125  &amp; CHAR(39) &amp; "," &amp; RIGHT($A126,1) &amp; ");","")</f>
@@ -2448,7 +2450,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A126  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A127,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A126,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A127,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C126" s="2" t="str">
@@ -2461,8 +2463,8 @@
         <v>126</v>
       </c>
       <c r="B127" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A127  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A128,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_batrider',65);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A127,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A128,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'batrider',65);</v>
       </c>
       <c r="C127" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A127  &amp; CHAR(39) &amp; "," &amp; RIGHT($A128,1) &amp; ");","")</f>
@@ -2474,7 +2476,7 @@
         <v>127</v>
       </c>
       <c r="B128" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A128  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A129,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A128,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A129,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C128" s="2" t="str">
@@ -2487,8 +2489,8 @@
         <v>128</v>
       </c>
       <c r="B129" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A129  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A130,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_chen',66);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A129,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A130,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'chen',66);</v>
       </c>
       <c r="C129" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A129  &amp; CHAR(39) &amp; "," &amp; RIGHT($A130,1) &amp; ");","")</f>
@@ -2500,7 +2502,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A130  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A131,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A130,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A131,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C130" s="2" t="str">
@@ -2513,8 +2515,8 @@
         <v>130</v>
       </c>
       <c r="B131" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A131  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A132,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_spectre',67);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A131,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A132,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'spectre',67);</v>
       </c>
       <c r="C131" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A131  &amp; CHAR(39) &amp; "," &amp; RIGHT($A132,1) &amp; ");","")</f>
@@ -2526,7 +2528,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A132  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A133,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A132,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A133,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C132" s="2" t="str">
@@ -2539,8 +2541,8 @@
         <v>132</v>
       </c>
       <c r="B133" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A133  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A134,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_doom_bringer',69);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A133,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A134,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'doom_bringer',69);</v>
       </c>
       <c r="C133" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A133  &amp; CHAR(39) &amp; "," &amp; RIGHT($A134,1) &amp; ");","")</f>
@@ -2552,7 +2554,7 @@
         <v>133</v>
       </c>
       <c r="B134" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A134  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A135,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A134,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A135,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C134" s="2" t="str">
@@ -2565,8 +2567,8 @@
         <v>134</v>
       </c>
       <c r="B135" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A135  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A136,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_ancient_apparition',68);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A135,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A136,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'ancient_apparition',68);</v>
       </c>
       <c r="C135" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A135  &amp; CHAR(39) &amp; "," &amp; RIGHT($A136,1) &amp; ");","")</f>
@@ -2578,7 +2580,7 @@
         <v>135</v>
       </c>
       <c r="B136" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A136  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A137,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A136,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A137,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C136" s="2" t="str">
@@ -2591,8 +2593,8 @@
         <v>136</v>
       </c>
       <c r="B137" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A137  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A138,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_ursa',70);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A137,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A138,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'ursa',70);</v>
       </c>
       <c r="C137" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A137  &amp; CHAR(39) &amp; "," &amp; RIGHT($A138,1) &amp; ");","")</f>
@@ -2604,7 +2606,7 @@
         <v>137</v>
       </c>
       <c r="B138" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A138  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A139,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A138,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A139,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C138" s="2" t="str">
@@ -2617,8 +2619,8 @@
         <v>138</v>
       </c>
       <c r="B139" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A139  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A140,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_spirit_breaker',71);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A139,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A140,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'spirit_breaker',71);</v>
       </c>
       <c r="C139" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A139  &amp; CHAR(39) &amp; "," &amp; RIGHT($A140,1) &amp; ");","")</f>
@@ -2630,7 +2632,7 @@
         <v>139</v>
       </c>
       <c r="B140" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A140  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A141,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A140,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A141,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C140" s="2" t="str">
@@ -2643,8 +2645,8 @@
         <v>140</v>
       </c>
       <c r="B141" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A141  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A142,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_gyrocopter',72);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A141,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A142,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'gyrocopter',72);</v>
       </c>
       <c r="C141" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A141  &amp; CHAR(39) &amp; "," &amp; RIGHT($A142,1) &amp; ");","")</f>
@@ -2656,7 +2658,7 @@
         <v>141</v>
       </c>
       <c r="B142" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A142  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A143,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A142,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A143,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C142" s="2" t="str">
@@ -2669,8 +2671,8 @@
         <v>142</v>
       </c>
       <c r="B143" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A143  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A144,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_alchemist',73);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A143,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A144,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'alchemist',73);</v>
       </c>
       <c r="C143" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A143  &amp; CHAR(39) &amp; "," &amp; RIGHT($A144,1) &amp; ");","")</f>
@@ -2682,7 +2684,7 @@
         <v>143</v>
       </c>
       <c r="B144" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A144  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A145,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A144,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A145,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C144" s="2" t="str">
@@ -2695,8 +2697,8 @@
         <v>144</v>
       </c>
       <c r="B145" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A145  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A146,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_invoker',74);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A145,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A146,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'invoker',74);</v>
       </c>
       <c r="C145" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A145  &amp; CHAR(39) &amp; "," &amp; RIGHT($A146,1) &amp; ");","")</f>
@@ -2708,7 +2710,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A146  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A147,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A146,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A147,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C146" s="2" t="str">
@@ -2721,8 +2723,8 @@
         <v>146</v>
       </c>
       <c r="B147" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A147  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A148,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_silencer',75);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A147,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A148,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'silencer',75);</v>
       </c>
       <c r="C147" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A147  &amp; CHAR(39) &amp; "," &amp; RIGHT($A148,1) &amp; ");","")</f>
@@ -2734,7 +2736,7 @@
         <v>147</v>
       </c>
       <c r="B148" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A148  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A149,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A148,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A149,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C148" s="2" t="str">
@@ -2747,8 +2749,8 @@
         <v>148</v>
       </c>
       <c r="B149" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A149  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A150,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_obsidian_destroyer',76);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A149,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A150,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'obsidian_destroyer',76);</v>
       </c>
       <c r="C149" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A149  &amp; CHAR(39) &amp; "," &amp; RIGHT($A150,1) &amp; ");","")</f>
@@ -2760,7 +2762,7 @@
         <v>149</v>
       </c>
       <c r="B150" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A150  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A151,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A150,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A151,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C150" s="2" t="str">
@@ -2773,8 +2775,8 @@
         <v>150</v>
       </c>
       <c r="B151" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A151  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A152,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_lycan',77);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A151,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A152,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'lycan',77);</v>
       </c>
       <c r="C151" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A151  &amp; CHAR(39) &amp; "," &amp; RIGHT($A152,1) &amp; ");","")</f>
@@ -2786,7 +2788,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A152  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A153,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A152,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A153,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C152" s="2" t="str">
@@ -2799,8 +2801,8 @@
         <v>152</v>
       </c>
       <c r="B153" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A153  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A154,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_brewmaster',78);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A153,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A154,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'brewmaster',78);</v>
       </c>
       <c r="C153" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A153  &amp; CHAR(39) &amp; "," &amp; RIGHT($A154,1) &amp; ");","")</f>
@@ -2812,7 +2814,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A154  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A155,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A154,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A155,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C154" s="2" t="str">
@@ -2825,8 +2827,8 @@
         <v>154</v>
       </c>
       <c r="B155" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A155  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A156,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_shadow_demon',79);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A155,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A156,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'shadow_demon',79);</v>
       </c>
       <c r="C155" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A155  &amp; CHAR(39) &amp; "," &amp; RIGHT($A156,1) &amp; ");","")</f>
@@ -2838,7 +2840,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A156  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A157,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A156,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A157,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C156" s="2" t="str">
@@ -2851,8 +2853,8 @@
         <v>156</v>
       </c>
       <c r="B157" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A157  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A158,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_lone_druid',80);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A157,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A158,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'lone_druid',80);</v>
       </c>
       <c r="C157" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A157  &amp; CHAR(39) &amp; "," &amp; RIGHT($A158,1) &amp; ");","")</f>
@@ -2864,7 +2866,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A158  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A159,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A158,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A159,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C158" s="2" t="str">
@@ -2877,8 +2879,8 @@
         <v>158</v>
       </c>
       <c r="B159" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A159  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A160,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_chaos_knight',81);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A159,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A160,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'chaos_knight',81);</v>
       </c>
       <c r="C159" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A159  &amp; CHAR(39) &amp; "," &amp; RIGHT($A160,1) &amp; ");","")</f>
@@ -2890,7 +2892,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A160  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A161,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A160,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A161,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C160" s="2" t="str">
@@ -2903,8 +2905,8 @@
         <v>160</v>
       </c>
       <c r="B161" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A161  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A162,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_meepo',82);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A161,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A162,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'meepo',82);</v>
       </c>
       <c r="C161" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A161  &amp; CHAR(39) &amp; "," &amp; RIGHT($A162,1) &amp; ");","")</f>
@@ -2916,7 +2918,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A162  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A163,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A162,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A163,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C162" s="2" t="str">
@@ -2929,8 +2931,8 @@
         <v>162</v>
       </c>
       <c r="B163" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A163  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A164,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_treant',83);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A163,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A164,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'treant',83);</v>
       </c>
       <c r="C163" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A163  &amp; CHAR(39) &amp; "," &amp; RIGHT($A164,1) &amp; ");","")</f>
@@ -2942,7 +2944,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A164  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A165,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A164,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A165,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C164" s="2" t="str">
@@ -2955,8 +2957,8 @@
         <v>164</v>
       </c>
       <c r="B165" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A165  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A166,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_ogre_magi',84);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A165,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A166,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'ogre_magi',84);</v>
       </c>
       <c r="C165" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A165  &amp; CHAR(39) &amp; "," &amp; RIGHT($A166,1) &amp; ");","")</f>
@@ -2968,7 +2970,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A166  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A167,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A166,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A167,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C166" s="2" t="str">
@@ -2981,8 +2983,8 @@
         <v>166</v>
       </c>
       <c r="B167" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A167  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A168,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_undying',85);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A167,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A168,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'undying',85);</v>
       </c>
       <c r="C167" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A167  &amp; CHAR(39) &amp; "," &amp; RIGHT($A168,1) &amp; ");","")</f>
@@ -2994,7 +2996,7 @@
         <v>167</v>
       </c>
       <c r="B168" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A168  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A169,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A168,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A169,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C168" s="2" t="str">
@@ -3007,8 +3009,8 @@
         <v>168</v>
       </c>
       <c r="B169" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A169  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A170,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_rubick',86);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A169,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A170,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'rubick',86);</v>
       </c>
       <c r="C169" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A169  &amp; CHAR(39) &amp; "," &amp; RIGHT($A170,1) &amp; ");","")</f>
@@ -3020,7 +3022,7 @@
         <v>169</v>
       </c>
       <c r="B170" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A170  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A171,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A170,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A171,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C170" s="2" t="str">
@@ -3033,8 +3035,8 @@
         <v>170</v>
       </c>
       <c r="B171" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A171  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A172,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_disruptor',87);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A171,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A172,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'disruptor',87);</v>
       </c>
       <c r="C171" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A171  &amp; CHAR(39) &amp; "," &amp; RIGHT($A172,1) &amp; ");","")</f>
@@ -3046,7 +3048,7 @@
         <v>171</v>
       </c>
       <c r="B172" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A172  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A173,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A172,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A173,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C172" s="2" t="str">
@@ -3059,8 +3061,8 @@
         <v>172</v>
       </c>
       <c r="B173" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A173  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A174,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_nyx_assassin',88);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A173,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A174,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'nyx_assassin',88);</v>
       </c>
       <c r="C173" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A173  &amp; CHAR(39) &amp; "," &amp; RIGHT($A174,1) &amp; ");","")</f>
@@ -3072,7 +3074,7 @@
         <v>173</v>
       </c>
       <c r="B174" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A174  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A175,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A174,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A175,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C174" s="2" t="str">
@@ -3085,8 +3087,8 @@
         <v>174</v>
       </c>
       <c r="B175" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A175  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A176,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_naga_siren',89);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A175,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A176,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'naga_siren',89);</v>
       </c>
       <c r="C175" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A175  &amp; CHAR(39) &amp; "," &amp; RIGHT($A176,1) &amp; ");","")</f>
@@ -3098,7 +3100,7 @@
         <v>175</v>
       </c>
       <c r="B176" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A176  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A177,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A176,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A177,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C176" s="2" t="str">
@@ -3111,8 +3113,8 @@
         <v>176</v>
       </c>
       <c r="B177" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A177  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A178,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_keeper_of_the_light',90);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A177,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A178,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'keeper_of_the_light',90);</v>
       </c>
       <c r="C177" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A177  &amp; CHAR(39) &amp; "," &amp; RIGHT($A178,1) &amp; ");","")</f>
@@ -3124,7 +3126,7 @@
         <v>177</v>
       </c>
       <c r="B178" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A178  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A179,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A178,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A179,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C178" s="2" t="str">
@@ -3137,8 +3139,8 @@
         <v>178</v>
       </c>
       <c r="B179" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A179  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A180,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_wisp',91);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A179,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A180,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'wisp',91);</v>
       </c>
       <c r="C179" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A179  &amp; CHAR(39) &amp; "," &amp; RIGHT($A180,1) &amp; ");","")</f>
@@ -3150,7 +3152,7 @@
         <v>179</v>
       </c>
       <c r="B180" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A180  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A181,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A180,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A181,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C180" s="2" t="str">
@@ -3163,8 +3165,8 @@
         <v>180</v>
       </c>
       <c r="B181" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A181  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A182,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_visage',92);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A181,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A182,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'visage',92);</v>
       </c>
       <c r="C181" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A181  &amp; CHAR(39) &amp; "," &amp; RIGHT($A182,1) &amp; ");","")</f>
@@ -3176,7 +3178,7 @@
         <v>181</v>
       </c>
       <c r="B182" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A182  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A183,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A182,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A183,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C182" s="2" t="str">
@@ -3189,8 +3191,8 @@
         <v>182</v>
       </c>
       <c r="B183" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A183  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A184,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_slark',93);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A183,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A184,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'slark',93);</v>
       </c>
       <c r="C183" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A183  &amp; CHAR(39) &amp; "," &amp; RIGHT($A184,1) &amp; ");","")</f>
@@ -3202,7 +3204,7 @@
         <v>183</v>
       </c>
       <c r="B184" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A184  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A185,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A184,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A185,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C184" s="2" t="str">
@@ -3215,8 +3217,8 @@
         <v>184</v>
       </c>
       <c r="B185" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A185  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A186,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_medusa',94);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A185,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A186,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'medusa',94);</v>
       </c>
       <c r="C185" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A185  &amp; CHAR(39) &amp; "," &amp; RIGHT($A186,1) &amp; ");","")</f>
@@ -3228,7 +3230,7 @@
         <v>185</v>
       </c>
       <c r="B186" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A186  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A187,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A186,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A187,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C186" s="2" t="str">
@@ -3241,8 +3243,8 @@
         <v>186</v>
       </c>
       <c r="B187" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A187  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A188,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_troll_warlord',95);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A187,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A188,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'troll_warlord',95);</v>
       </c>
       <c r="C187" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A187  &amp; CHAR(39) &amp; "," &amp; RIGHT($A188,1) &amp; ");","")</f>
@@ -3254,7 +3256,7 @@
         <v>187</v>
       </c>
       <c r="B188" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A188  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A189,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A188,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A189,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C188" s="2" t="str">
@@ -3267,8 +3269,8 @@
         <v>188</v>
       </c>
       <c r="B189" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A189  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A190,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_centaur',96);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A189,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A190,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'centaur',96);</v>
       </c>
       <c r="C189" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A189  &amp; CHAR(39) &amp; "," &amp; RIGHT($A190,1) &amp; ");","")</f>
@@ -3280,7 +3282,7 @@
         <v>189</v>
       </c>
       <c r="B190" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A190  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A191,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A190,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A191,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C190" s="2" t="str">
@@ -3293,8 +3295,8 @@
         <v>190</v>
       </c>
       <c r="B191" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A191  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A192,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_magnataur',97);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A191,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A192,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'magnataur',97);</v>
       </c>
       <c r="C191" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A191  &amp; CHAR(39) &amp; "," &amp; RIGHT($A192,1) &amp; ");","")</f>
@@ -3306,7 +3308,7 @@
         <v>191</v>
       </c>
       <c r="B192" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A192  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A193,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A192,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A193,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C192" s="2" t="str">
@@ -3319,8 +3321,8 @@
         <v>192</v>
       </c>
       <c r="B193" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A193  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A194,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_shredder',98);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A193,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A194,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'shredder',98);</v>
       </c>
       <c r="C193" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A193  &amp; CHAR(39) &amp; "," &amp; RIGHT($A194,1) &amp; ");","")</f>
@@ -3332,7 +3334,7 @@
         <v>193</v>
       </c>
       <c r="B194" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A194  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A195,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A194,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A195,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C194" s="2" t="str">
@@ -3345,8 +3347,8 @@
         <v>194</v>
       </c>
       <c r="B195" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A195  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A196,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_bristleback',99);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A195,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A196,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'bristleback',99);</v>
       </c>
       <c r="C195" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A195  &amp; CHAR(39) &amp; "," &amp; RIGHT($A196,1) &amp; ");","")</f>
@@ -3358,7 +3360,7 @@
         <v>195</v>
       </c>
       <c r="B196" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A196  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A197,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A196,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A197,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C196" s="2" t="str">
@@ -3371,8 +3373,8 @@
         <v>196</v>
       </c>
       <c r="B197" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A197  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A198,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_tusk',100);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A197,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A198,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'tusk',100);</v>
       </c>
       <c r="C197" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A197  &amp; CHAR(39) &amp; "," &amp; RIGHT($A198,1) &amp; ");","")</f>
@@ -3384,7 +3386,7 @@
         <v>197</v>
       </c>
       <c r="B198" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A198  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A199,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A198,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A199,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C198" s="2" t="str">
@@ -3397,8 +3399,8 @@
         <v>198</v>
       </c>
       <c r="B199" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A199  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A200,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_skywrath_mage',101);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A199,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A200,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'skywrath_mage',101);</v>
       </c>
       <c r="C199" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A199  &amp; CHAR(39) &amp; "," &amp; RIGHT($A200,1) &amp; ");","")</f>
@@ -3410,7 +3412,7 @@
         <v>199</v>
       </c>
       <c r="B200" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A200  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A201,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A200,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A201,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C200" s="2" t="str">
@@ -3423,8 +3425,8 @@
         <v>200</v>
       </c>
       <c r="B201" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A201  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A202,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_abaddon',102);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A201,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A202,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'abaddon',102);</v>
       </c>
       <c r="C201" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A201  &amp; CHAR(39) &amp; "," &amp; RIGHT($A202,1) &amp; ");","")</f>
@@ -3436,7 +3438,7 @@
         <v>201</v>
       </c>
       <c r="B202" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A202  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A203,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A202,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A203,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C202" s="2" t="str">
@@ -3449,8 +3451,8 @@
         <v>202</v>
       </c>
       <c r="B203" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A203  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A204,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_elder_titan',103);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A203,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A204,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'elder_titan',103);</v>
       </c>
       <c r="C203" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A203  &amp; CHAR(39) &amp; "," &amp; RIGHT($A204,1) &amp; ");","")</f>
@@ -3462,7 +3464,7 @@
         <v>203</v>
       </c>
       <c r="B204" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A204  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A205,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A204,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A205,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C204" s="2" t="str">
@@ -3475,8 +3477,8 @@
         <v>204</v>
       </c>
       <c r="B205" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A205  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A206,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_legion_commander',104);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A205,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A206,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'legion_commander',104);</v>
       </c>
       <c r="C205" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A205  &amp; CHAR(39) &amp; "," &amp; RIGHT($A206,1) &amp; ");","")</f>
@@ -3488,7 +3490,7 @@
         <v>205</v>
       </c>
       <c r="B206" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A206  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A207,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A206,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A207,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C206" s="2" t="str">
@@ -3501,8 +3503,8 @@
         <v>206</v>
       </c>
       <c r="B207" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A207  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A208,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_ember_spirit',106);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A207,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A208,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'ember_spirit',106);</v>
       </c>
       <c r="C207" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A207  &amp; CHAR(39) &amp; "," &amp; RIGHT($A208,1) &amp; ");","")</f>
@@ -3514,7 +3516,7 @@
         <v>207</v>
       </c>
       <c r="B208" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A208  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A209,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A208,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A209,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C208" s="2" t="str">
@@ -3527,8 +3529,8 @@
         <v>208</v>
       </c>
       <c r="B209" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A209  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A210,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_earth_spirit',107);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A209,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A210,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'earth_spirit',107);</v>
       </c>
       <c r="C209" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A209  &amp; CHAR(39) &amp; "," &amp; RIGHT($A210,1) &amp; ");","")</f>
@@ -3540,7 +3542,7 @@
         <v>209</v>
       </c>
       <c r="B210" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A210  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A211,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A210,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A211,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C210" s="2" t="str">
@@ -3553,8 +3555,8 @@
         <v>210</v>
       </c>
       <c r="B211" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A211  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A212,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_terrorblade',109);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A211,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A212,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'terrorblade',109);</v>
       </c>
       <c r="C211" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A211  &amp; CHAR(39) &amp; "," &amp; RIGHT($A212,1) &amp; ");","")</f>
@@ -3566,7 +3568,7 @@
         <v>211</v>
       </c>
       <c r="B212" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A212  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A213,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A212,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A213,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C212" s="2" t="str">
@@ -3579,8 +3581,8 @@
         <v>212</v>
       </c>
       <c r="B213" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A213  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A214,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_phoenix',110);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A213,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A214,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'phoenix',110);</v>
       </c>
       <c r="C213" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A213  &amp; CHAR(39) &amp; "," &amp; RIGHT($A214,1) &amp; ");","")</f>
@@ -3592,7 +3594,7 @@
         <v>213</v>
       </c>
       <c r="B214" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A214  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A215,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A214,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A215,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C214" s="2" t="str">
@@ -3605,8 +3607,8 @@
         <v>214</v>
       </c>
       <c r="B215" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A215  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A216,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_oracle',111);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A215,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A216,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'oracle',111);</v>
       </c>
       <c r="C215" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A215  &amp; CHAR(39) &amp; "," &amp; RIGHT($A216,1) &amp; ");","")</f>
@@ -3618,7 +3620,7 @@
         <v>215</v>
       </c>
       <c r="B216" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A216  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A217,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A216,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A217,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C216" s="2" t="str">
@@ -3631,8 +3633,8 @@
         <v>216</v>
       </c>
       <c r="B217" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A217  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A218,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_techies',105);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A217,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A218,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'techies',105);</v>
       </c>
       <c r="C217" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A217  &amp; CHAR(39) &amp; "," &amp; RIGHT($A218,1) &amp; ");","")</f>
@@ -3644,7 +3646,7 @@
         <v>217</v>
       </c>
       <c r="B218" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A218  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A219,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A218,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A219,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C218" s="2" t="str">
@@ -3657,8 +3659,8 @@
         <v>218</v>
       </c>
       <c r="B219" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A219  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A220,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_winter_wyvern',112);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A219,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A220,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'winter_wyvern',112);</v>
       </c>
       <c r="C219" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A219  &amp; CHAR(39) &amp; "," &amp; RIGHT($A220,1) &amp; ");","")</f>
@@ -3670,7 +3672,7 @@
         <v>219</v>
       </c>
       <c r="B220" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A220  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A221,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A220,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A221,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C220" s="2" t="str">
@@ -3683,8 +3685,8 @@
         <v>220</v>
       </c>
       <c r="B221" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A221  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A222,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_arc_warden',113);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A221,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A222,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'arc_warden',113);</v>
       </c>
       <c r="C221" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A221  &amp; CHAR(39) &amp; "," &amp; RIGHT($A222,1) &amp; ");","")</f>
@@ -3696,7 +3698,7 @@
         <v>221</v>
       </c>
       <c r="B222" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A222  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A223,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A222,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A223,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C222" s="2" t="str">
@@ -3709,8 +3711,8 @@
         <v>222</v>
       </c>
       <c r="B223" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A223  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A224,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_abyssal_underlord',108);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A223,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A224,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'abyssal_underlord',108);</v>
       </c>
       <c r="C223" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A223  &amp; CHAR(39) &amp; "," &amp; RIGHT($A224,1) &amp; ");","")</f>
@@ -3722,7 +3724,7 @@
         <v>223</v>
       </c>
       <c r="B224" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A224  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A225,"ID: ","") &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A224,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A225,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
       <c r="C224" s="2" t="str">
@@ -3735,8 +3737,8 @@
         <v>224</v>
       </c>
       <c r="B225" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A225  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A226,"ID: ","") &amp; ");","")</f>
-        <v>Insert into Heroes ('name','valveid') values ( 'Hero: npc_dota_hero_monkey_king',114);</v>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A225,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A226,"ID: ","") &amp; ");","")</f>
+        <v>Insert into Heroes (name,valveid) values ( 'monkey_king',114);</v>
       </c>
       <c r="C225" s="2" t="str">
         <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A225  &amp; CHAR(39) &amp; "," &amp; RIGHT($A226,1) &amp; ");","")</f>
@@ -3748,7 +3750,7 @@
         <v>225</v>
       </c>
       <c r="B226" s="2" t="str">
-        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; CHAR(39) &amp; "name" &amp; CHAR(39) &amp; "," &amp; CHAR(39) &amp; "valveid" &amp; CHAR(39) &amp; ") values ( " &amp; CHAR(39) &amp; $A226  &amp; CHAR(39) &amp; "," &amp; RIGHT($A227,1) &amp; ");","")</f>
+        <f aca="false">IF(MOD(ROW(),2),"Insert into Heroes (" &amp; "name" &amp; "," &amp; "valveid" &amp; ") values ( " &amp; CHAR(39) &amp; SUBSTITUTE($A226,"Hero: npc_dota_hero_","")  &amp; CHAR(39) &amp; "," &amp; SUBSTITUTE($A227,"ID: ","") &amp; ");","")</f>
         <v/>
       </c>
     </row>

</xml_diff>